<commit_message>
update to phase 2
</commit_message>
<xml_diff>
--- a/phase_2_all_models_results.xlsx
+++ b/phase_2_all_models_results.xlsx
@@ -523,10 +523,10 @@
         <v>1.037873121739411e-07</v>
       </c>
       <c r="J2" t="n">
-        <v>1.116021560731529e-10</v>
+        <v>1.11722290685571e-10</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1319101748798834</v>
+        <v>0.1319101748798887</v>
       </c>
     </row>
     <row r="3">
@@ -560,10 +560,10 @@
         <v>1.941421124230497</v>
       </c>
       <c r="J3" t="n">
-        <v>1.572967933766973</v>
+        <v>54.50398119811268</v>
       </c>
       <c r="K3" t="n">
-        <v>0.6537582844693701</v>
+        <v>2.689612997095686</v>
       </c>
     </row>
     <row r="4">
@@ -597,10 +597,10 @@
         <v>11.07525535541896</v>
       </c>
       <c r="J4" t="n">
-        <v>6.887531083428539</v>
+        <v>45.76948907227623</v>
       </c>
       <c r="K4" t="n">
-        <v>1.379807284223116</v>
+        <v>2.59299930514257</v>
       </c>
     </row>
     <row r="5">
@@ -634,10 +634,10 @@
         <v>1.672439235256276</v>
       </c>
       <c r="J5" t="n">
-        <v>1.330706197781046</v>
+        <v>57.62401814901956</v>
       </c>
       <c r="K5" t="n">
-        <v>0.6253260842914143</v>
+        <v>2.806510561970689</v>
       </c>
     </row>
     <row r="6">
@@ -671,10 +671,10 @@
         <v>1.422818947696345</v>
       </c>
       <c r="J6" t="n">
-        <v>1.121006538306673</v>
+        <v>51.77132656569123</v>
       </c>
       <c r="K6" t="n">
-        <v>0.4859350813637881</v>
+        <v>2.519071808760003</v>
       </c>
     </row>
     <row r="7">
@@ -708,10 +708,10 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>69.83177860377482</v>
       </c>
       <c r="K7" t="n">
-        <v>0.00273972602739726</v>
+        <v>3.643227801463834</v>
       </c>
     </row>
   </sheetData>
@@ -1164,13 +1164,13 @@
         <v>1.335506583153352e-12</v>
       </c>
       <c r="F12" t="n">
-        <v>2.08157047201149e-08</v>
+        <v>2.083811187340613e-08</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>2.08157047201149e-08</v>
+        <v>2.083811187340613e-08</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -1178,7 +1178,7 @@
         </is>
       </c>
       <c r="J12" t="n">
-        <v>1.116021560731529e-10</v>
+        <v>1.11722290685571e-10</v>
       </c>
     </row>
     <row r="13">
@@ -1560,13 +1560,13 @@
         <v>0.01882319396462151</v>
       </c>
       <c r="F23" t="n">
-        <v>293.3853358714736</v>
+        <v>10165.92168655722</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>293.3853358714736</v>
+        <v>10165.92168655722</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -1574,7 +1574,7 @@
         </is>
       </c>
       <c r="J23" t="n">
-        <v>1.572967933766973</v>
+        <v>54.50398119811268</v>
       </c>
     </row>
     <row r="24">
@@ -1956,13 +1956,13 @@
         <v>0.08242083690177843</v>
       </c>
       <c r="F34" t="n">
-        <v>1284.641966856682</v>
+        <v>8536.789997986572</v>
       </c>
       <c r="G34" t="n">
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>1284.641966856682</v>
+        <v>8536.789997986572</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
@@ -1970,7 +1970,7 @@
         </is>
       </c>
       <c r="J34" t="n">
-        <v>6.887531083428539</v>
+        <v>45.76948907227623</v>
       </c>
     </row>
     <row r="35">
@@ -2352,13 +2352,13 @@
         <v>0.01592412682613997</v>
       </c>
       <c r="F45" t="n">
-        <v>248.1993919909628</v>
+        <v>10747.8617688201</v>
       </c>
       <c r="G45" t="n">
         <v>0</v>
       </c>
       <c r="H45" t="n">
-        <v>248.1993919909628</v>
+        <v>10747.8617688201</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
@@ -2366,7 +2366,7 @@
         </is>
       </c>
       <c r="J45" t="n">
-        <v>1.330706197781046</v>
+        <v>57.62401814901956</v>
       </c>
     </row>
     <row r="46">
@@ -2748,13 +2748,13 @@
         <v>0.01341471943145245</v>
       </c>
       <c r="F56" t="n">
-        <v>209.0868305036561</v>
+        <v>9656.235010851295</v>
       </c>
       <c r="G56" t="n">
         <v>0</v>
       </c>
       <c r="H56" t="n">
-        <v>209.0868305036561</v>
+        <v>9656.235010851295</v>
       </c>
       <c r="I56" t="inlineStr">
         <is>
@@ -2762,7 +2762,7 @@
         </is>
       </c>
       <c r="J56" t="n">
-        <v>1.121006538306673</v>
+        <v>51.77132656569123</v>
       </c>
     </row>
     <row r="57">
@@ -3144,13 +3144,13 @@
         <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>0</v>
+        <v>13024.81721360125</v>
       </c>
       <c r="G67" t="n">
         <v>0</v>
       </c>
       <c r="H67" t="n">
-        <v>0</v>
+        <v>13024.81721360125</v>
       </c>
       <c r="I67" t="inlineStr">
         <is>
@@ -3158,7 +3158,7 @@
         </is>
       </c>
       <c r="J67" t="n">
-        <v>0</v>
+        <v>69.83177860377482</v>
       </c>
     </row>
   </sheetData>
@@ -3200,40 +3200,40 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>KaplanMeier</t>
+          <t>Flat</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1284.641966856682</v>
+        <v>13024.81721360125</v>
       </c>
       <c r="C2" t="n">
-        <v>6.887531083428539</v>
+        <v>69.83177860377482</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Weibull</t>
+          <t>LogNormal</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>293.3853358714736</v>
+        <v>10747.8617688201</v>
       </c>
       <c r="C3" t="n">
-        <v>1.572967933766973</v>
+        <v>57.62401814901956</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>LogNormal</t>
+          <t>Weibull</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>248.1993919909628</v>
+        <v>10165.92168655722</v>
       </c>
       <c r="C4" t="n">
-        <v>1.330706197781046</v>
+        <v>54.50398119811268</v>
       </c>
     </row>
     <row r="5">
@@ -3243,36 +3243,36 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>209.0868305036561</v>
+        <v>9656.235010851295</v>
       </c>
       <c r="C5" t="n">
-        <v>1.121006538306673</v>
+        <v>51.77132656569123</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Exponential</t>
+          <t>KaplanMeier</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.08157047201149e-08</v>
+        <v>8536.789997986572</v>
       </c>
       <c r="C6" t="n">
-        <v>1.116021560731529e-10</v>
+        <v>45.76948907227623</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Flat</t>
+          <t>Exponential</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>2.083811187340613e-08</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>1.11722290685571e-10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>